<commit_message>
Contest Adder Final From
Edit Functionality to read from excel and create events
</commit_message>
<xml_diff>
--- a/Contest Adder(Google Calander API)/CodeforceCalander.xlsx
+++ b/Contest Adder(Google Calander API)/CodeforceCalander.xlsx
@@ -13,7 +13,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
-    <t xml:space="preserve"> Name</t>
+    <t>Name</t>
   </si>
   <si>
     <t>Start</t>
@@ -85,15 +85,21 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -103,16 +109,78 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -122,23 +190,38 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="20" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="21" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -158,6 +241,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -357,17 +441,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -394,10 +478,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -636,12 +720,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -918,7 +1002,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -945,10 +1029,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1190,7 +1274,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1198,8 +1282,8 @@
   <cols>
     <col min="1" max="1" width="33.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.6719" style="1" customWidth="1"/>
-    <col min="3" max="6" width="8.85156" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="3" max="5" width="8.85156" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1213,8 +1297,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
@@ -1223,12 +1306,11 @@
       <c r="B2" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="C2" s="4">
-        <v>1.083333333333333</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="C2" s="5">
+        <v>4.083333333333333</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="2">
@@ -1237,12 +1319,11 @@
       <c r="B3" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="C3" s="4">
-        <v>1.083333333333333</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="C3" s="5">
+        <v>4.083333333333333</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
       <c r="A4" t="s" s="2">
@@ -1251,12 +1332,11 @@
       <c r="B4" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="C4" s="4">
-        <v>1.083333333333333</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="C4" s="5">
+        <v>4.083333333333333</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" t="s" s="2">
@@ -1265,12 +1345,11 @@
       <c r="B5" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="C5" s="4">
-        <v>1.083333333333333</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="C5" s="5">
+        <v>4.083333333333333</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" t="s" s="2">
@@ -1279,12 +1358,11 @@
       <c r="B6" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="C6" s="4">
-        <v>1.104166666666667</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="C6" s="5">
+        <v>4.104166666666667</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" t="s" s="2">
@@ -1293,12 +1371,11 @@
       <c r="B7" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="C7" s="4">
-        <v>1.104166666666667</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="C7" s="5">
+        <v>4.104166666666667</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" t="s" s="2">
@@ -1307,12 +1384,11 @@
       <c r="B8" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="C8" s="4">
-        <v>1.083333333333333</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="C8" s="5">
+        <v>4.083333333333333</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" t="s" s="2">
@@ -1321,12 +1397,11 @@
       <c r="B9" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="C9" s="4">
-        <v>1.083333333333333</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="C9" s="5">
+        <v>4.083333333333333</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" t="s" s="2">
@@ -1335,12 +1410,11 @@
       <c r="B10" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="C10" s="4">
-        <v>1.083333333333333</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="C10" s="5">
+        <v>4.083333333333333</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" ht="13.55" customHeight="1">
       <c r="A11" t="s" s="2">
@@ -1349,45 +1423,13 @@
       <c r="B11" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="C11" s="5">
-        <v>1.583333333333333</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" ht="13.55" customHeight="1">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="C11" s="8">
+        <v>4.583333333333333</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>